<commit_message>
Remote Indigenous Housing - state views.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
+++ b/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t xml:space="preserve">NPARIH capital works progress, number of new houses and refurbishments, by state and territory, 2008-2015 </t>
   </si>
@@ -77,22 +77,46 @@
     <t xml:space="preserve">Other Benchmarks</t>
   </si>
   <si>
-    <t xml:space="preserve">Under NPARIH, states and the Northern Territory have a 20 per cent Indigenous employment target for capital works.  Over the life of NPARIH, all jurisdictions have met or exceeded this target. In addition, the Northern Territory Government has consistently delivered against a 40 per cent Indigenous employment target for property management and a 40 per cent Indigenous employment target for tenancy management, as outlined in the Northern Territory’s 2014- 16 Implementation Plan to the NPARIH.</t>
+    <t xml:space="preserve">Under NPARIH, states and the Northern Territory have a 20 per cent Indigenous employment target for capital works.  Over the life of NPARIH, all jurisdictions have met or exceeded this target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPARIH notional targets extend to 2014 for refurbishments and to 2018 for new build houses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victoria is not included in these analyses as no Commonwealth funding was provided to Victoria under the NPARIH for the construction of new houses or refurbishment of existing stock.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victoria and Tasmania are not currently a part of NPARIH as they exited in 2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACT does not participate in this agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victoria existed this agreement in 2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasmania exited this agreement in 2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Northern Territory Government has consistently delivered against a 40 per cent Indigenous employment target for property management and a 40 per cent Indigenous employment target for tenancy management, as outlined in the Northern Territory’s 2014-16 Implementation Plan to the NPARIH.</t>
   </si>
   <si>
     <t xml:space="preserve">Queensland has consistently exceeded the 20 per cent Indigenous employment target for capital works, with over 85 per cent of all available jobs in construction, repairs and maintenance during 2014-15 undertaken by Aboriginal and Torres Strait Islander workers.</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPARIH notional targets extend to 2014 for refurbishments and to 2018 for new build houses.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victoria is not included in these analyses as no Commonwealth funding was provided to Victoria under the NPARIH for the construction of new houses or refurbishment of existing stock.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victoria and Tasmania are not currently a part of NPARIH as they exited in 2014.</t>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In addition, the Northern Territory Government has consistently delivered against a 40 per cent Indigenous employment target for property management and a 40 per cent Indigenous employment target for tenancy management, as outlined in the Northern Territory’s 2014-16 Implementation Plan to the NPARIH.</t>
   </si>
 </sst>
 </file>
@@ -105,11 +129,12 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,12 +150,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -178,6 +197,7 @@
       <sz val="10"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,7 +217,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,20 +236,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,11 +253,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,31 +265,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,16 +298,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Microsoft Excel found an error in the formula you entered. Do you want to accept the correction proposed below?&#10;&#10;|&#10;&#10;• To accept the correction, click Yes.&#10;• To close this message and correct the formula yourself, click No. 16 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal_AIHW RoGS indicator concordance_NHA PI 13 4 yo health check" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 152" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -311,9 +323,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -443,7 +455,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -456,17 +468,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,7 +510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>17</v>
       </c>
@@ -506,33 +518,81 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="B6" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Remote Housing widget updates.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
+++ b/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
-  <si>
-    <t xml:space="preserve">NPARIH capital works progress, number of new houses and refurbishments, by state and territory, 2008-2015 </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">NPARIH capital works progress, number of new houses and refurbishments, by state and territory, 2008-2016 </t>
   </si>
   <si>
     <t xml:space="preserve">NSW</t>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Aust</t>
   </si>
   <si>
-    <t xml:space="preserve">New</t>
+    <t xml:space="preserve">New houses</t>
   </si>
   <si>
     <t xml:space="preserve">Refurbishments</t>
@@ -56,6 +56,18 @@
     <t xml:space="preserve">`</t>
   </si>
   <si>
+    <t xml:space="preserve">Measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,200 new houses to be delivered by 2018; 4,800 refurbishments to be delivered by 2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">short title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construction and refurbishment of homes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Status</t>
   </si>
   <si>
@@ -68,55 +80,58 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">Since the commencement of NPARIH to the end of October 2015, a total of 2,957 new houses have been delivered against the COAG new house target.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A total of 7,206 refurbishments have been delivered, considerably exceeding the COAG refurbishment target.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Benchmarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Under NPARIH, states and the Northern Territory have a 20 per cent Indigenous employment target for capital works.  Over the life of NPARIH, all jurisdictions have met or exceeded this target.</t>
+    <t xml:space="preserve">From 2008 to the end of October 2015, the NPRH and NPARIH delivered a total of 3,272 new houses against the 2018 COAG target of 4,200.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A total of 7,350 refurbishments were delivered, considerably exceeding the 2018 COAG target of 4800.</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">NPARIH notional targets extend to 2014 for refurbishments and to 2018 for new build houses.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Victoria is not included in these analyses as no Commonwealth funding was provided to Victoria under the NPARIH for the construction of new houses or refurbishment of existing stock.</t>
   </si>
   <si>
-    <t xml:space="preserve">Victoria and Tasmania are not currently a part of NPARIH as they exited in 2014.</t>
+    <t xml:space="preserve">Victoria and Tasmania exited the NPARIH in 2014 and are not part of the Remote Housing Strategy.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">New South Wales exited the NPARIH in 2015 and is not part of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Remote Housing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Strategy</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ACT</t>
   </si>
   <si>
-    <t xml:space="preserve">ACT does not participate in this agreement</t>
+    <t xml:space="preserve">The ACT does not participate in this National Partnership Agreement.</t>
   </si>
   <si>
     <t xml:space="preserve">Vic</t>
   </si>
   <si>
-    <t xml:space="preserve">Victoria existed this agreement in 2014.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tasmania exited this agreement in 2014.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Northern Territory Government has consistently delivered against a 40 per cent Indigenous employment target for property management and a 40 per cent Indigenous employment target for tenancy management, as outlined in the Northern Territory’s 2014-16 Implementation Plan to the NPARIH.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Queensland has consistently exceeded the 20 per cent Indigenous employment target for capital works, with over 85 per cent of all available jobs in construction, repairs and maintenance during 2014-15 undertaken by Aboriginal and Torres Strait Islander workers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In addition, the Northern Territory Government has consistently delivered against a 40 per cent Indigenous employment target for property management and a 40 per cent Indigenous employment target for tenancy management, as outlined in the Northern Territory’s 2014-16 Implementation Plan to the NPARIH.</t>
+    <t xml:space="preserve">Victoria does not participate in this National Partnership Agreement.</t>
   </si>
 </sst>
 </file>
@@ -129,7 +144,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,6 +195,19 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -187,17 +215,23 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -248,7 +282,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,10 +308,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,7 +315,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,7 +323,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -307,6 +353,66 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF00000A"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -315,20 +421,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -342,107 +446,105 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="n">
-        <v>241</v>
-      </c>
-      <c r="F4" s="8" t="n">
-        <v>653</v>
-      </c>
-      <c r="G4" s="8" t="n">
-        <v>622</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>235</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="C4" s="7" t="n">
+        <v>263</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>836</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>708</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>239</v>
+      </c>
+      <c r="G4" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="J4" s="8" t="n">
-        <v>1149</v>
-      </c>
-      <c r="K4" s="8" t="n">
-        <v>2912</v>
-      </c>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="6"/>
-      <c r="D5" s="7" t="s">
+      <c r="H4" s="7" t="n">
+        <v>1214</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>3272</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="n">
-        <v>1003</v>
-      </c>
-      <c r="F5" s="8" t="n">
+      <c r="C5" s="7" t="n">
+        <v>1009</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <v>1490</v>
       </c>
-      <c r="G5" s="8" t="n">
-        <v>1440</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>286</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="E5" s="7" t="n">
+        <v>1561</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>304</v>
+      </c>
+      <c r="G5" s="7" t="n">
         <v>57</v>
       </c>
-      <c r="J5" s="8" t="n">
+      <c r="H5" s="7" t="n">
         <v>2929</v>
       </c>
-      <c r="K5" s="8" t="n">
-        <v>7205</v>
-      </c>
-      <c r="M5" s="3"/>
+      <c r="I5" s="7" t="n">
+        <v>7350</v>
+      </c>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
+      <c r="A6" s="8"/>
       <c r="C6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="M6" s="3"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -451,7 +553,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -468,79 +570,78 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="62.6377551020408"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="11" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11" t="s">
+    <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11" t="s">
+      <c r="B7" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -548,45 +649,16 @@
       <c r="A10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remote housing NPA widgets: new widgets and fixes
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
+++ b/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
@@ -100,6 +100,7 @@
         <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">New South Wales exited the NPARIH in 2015 and is not part of the </t>
     </r>
@@ -117,6 +118,7 @@
         <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Strategy</t>
     </r>
@@ -232,6 +234,7 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -424,12 +427,14 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -573,13 +578,14 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="62.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="61.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Data and wording tweaks requested by Queensland apparently.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
+++ b/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">NPARIH capital works progress, number of new houses and refurbishments, by state and territory, 2008-2016 </t>
   </si>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">From 2008 to the end of October 2015, the NPRH and NPARIH delivered a total of 3,272 new houses against the 2018 COAG target of 4,200.</t>
+    <t xml:space="preserve">From 2008 to the end of October 2016, the NPRH and NPARIH delivered a total of 3,269 new houses against the 2018 COAG target of 4,200.</t>
   </si>
   <si>
     <t xml:space="preserve">A total of 7,350 refurbishments were delivered, considerably exceeding the 2018 COAG target of 4800.</t>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">New South Wales exited the NPARIH in 2015 and is not part of the NPRH.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totals include dwellings built from Commonwealth Own Purpose Expense funding under NPARIH.</t>
   </si>
   <si>
     <t xml:space="preserve">ACT</t>
@@ -600,8 +603,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -665,7 +668,7 @@
         <v>263</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="E4" s="7" t="n">
         <v>708</v>
@@ -680,7 +683,7 @@
         <v>1214</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>3272</v>
+        <v>3269</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -749,10 +752,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -794,7 +797,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
@@ -825,33 +828,38 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="10" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="10" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>